<commit_message>
changed order of header row in non-functional requirement
</commit_message>
<xml_diff>
--- a/input/system-requirements/CCC DAK_functional and non-functional requirements.xlsx
+++ b/input/system-requirements/CCC DAK_functional and non-functional requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/EmCare-External/Shared Documents/Em Care External/WS2 - Digital Adaptation Kit/1_global/copy edited/v1.8/ccc web annexes v1.8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/litlfred/space_cats/smart-dak-ccc/input/system-requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{385F10DC-8292-40B1-A7BD-E52C75EEC209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ECA1BF0-9E2F-481E-AEE7-72A710ADEF3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3B11C2-9E7B-6E4A-A1CD-96D8EB04F3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{05A1CA60-BB51-42D1-B0C0-680AB865CD46}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{05A1CA60-BB51-42D1-B0C0-680AB865CD46}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -8315,7 +8315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8994,6 +8994,24 @@
     <xf numFmtId="0" fontId="29" fillId="13" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -9010,24 +9028,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9113,7 +9113,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="OVERVIEW"/>
@@ -9162,9 +9162,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9202,7 +9202,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9308,7 +9308,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9450,7 +9450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9463,232 +9463,238 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="54" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="54" customWidth="1"/>
     <col min="2" max="2" width="10" style="54" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="54" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" style="54" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="54"/>
+    <col min="3" max="3" width="18.5" style="54" customWidth="1"/>
+    <col min="4" max="4" width="62.1640625" style="54" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="54" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="53"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="53"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="53"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="53"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="53"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="53"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-    </row>
-    <row r="9" spans="1:5" ht="62.25" customHeight="1">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+    </row>
+    <row r="9" spans="1:5" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="53"/>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-    </row>
-    <row r="10" spans="1:5" ht="21" customHeight="1" thickBot="1">
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+    </row>
+    <row r="10" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53"/>
       <c r="B10" s="53"/>
       <c r="C10" s="53"/>
       <c r="D10" s="55"/>
       <c r="E10" s="56"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="11" spans="1:5" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53"/>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="73" t="s">
         <v>500</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="67" t="s">
+      <c r="C11" s="74"/>
+      <c r="D11" s="73" t="s">
         <v>501</v>
       </c>
-      <c r="E11" s="68"/>
-    </row>
-    <row r="12" spans="1:5" ht="69.75" customHeight="1" thickTop="1" thickBot="1">
+      <c r="E11" s="74"/>
+    </row>
+    <row r="12" spans="1:5" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53"/>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="75" t="s">
         <v>502</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="71" t="s">
+      <c r="C12" s="76"/>
+      <c r="D12" s="65" t="s">
         <v>503</v>
       </c>
-      <c r="E12" s="72"/>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E12" s="66"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53"/>
       <c r="B13" s="57"/>
       <c r="C13" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="E13" s="72"/>
-    </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1">
+      <c r="E13" s="66"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="53"/>
       <c r="B14" s="59"/>
       <c r="C14" s="60" t="s">
         <v>505</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="65" t="s">
         <v>506</v>
       </c>
-      <c r="E14" s="72"/>
-    </row>
-    <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E14" s="66"/>
+    </row>
+    <row r="15" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53"/>
       <c r="B15" s="59"/>
       <c r="C15" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="65" t="s">
         <v>507</v>
       </c>
-      <c r="E15" s="72"/>
-    </row>
-    <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E15" s="66"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="59"/>
       <c r="C16" s="58" t="s">
         <v>508</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="65" t="s">
         <v>509</v>
       </c>
-      <c r="E16" s="72"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E16" s="66"/>
+    </row>
+    <row r="17" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
       <c r="B17" s="61"/>
       <c r="C17" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="65" t="s">
         <v>510</v>
       </c>
-      <c r="E17" s="72"/>
-    </row>
-    <row r="18" spans="1:5" ht="64.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="E17" s="66"/>
+    </row>
+    <row r="18" spans="1:5" ht="64.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="69" t="s">
         <v>511</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="71" t="s">
+      <c r="C18" s="70"/>
+      <c r="D18" s="65" t="s">
         <v>512</v>
       </c>
-      <c r="E18" s="72"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="E18" s="66"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="53"/>
       <c r="B19" s="57"/>
       <c r="C19" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="65" t="s">
         <v>513</v>
       </c>
-      <c r="E19" s="72"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="E19" s="66"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="53"/>
       <c r="B20" s="59"/>
       <c r="C20" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="65" t="s">
         <v>514</v>
       </c>
-      <c r="E20" s="72"/>
-    </row>
-    <row r="21" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
+      <c r="E20" s="66"/>
+    </row>
+    <row r="21" spans="1:5" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="53"/>
       <c r="B21" s="59"/>
       <c r="C21" s="62" t="s">
         <v>515</v>
       </c>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="65" t="s">
         <v>516</v>
       </c>
-      <c r="E21" s="72"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickTop="1">
+      <c r="E21" s="66"/>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53"/>
       <c r="B22" s="53"/>
       <c r="D22" s="53"/>
       <c r="E22" s="53"/>
     </row>
-    <row r="23" spans="1:5" ht="31.5" customHeight="1">
+    <row r="23" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="63"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="67" t="s">
         <v>519</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="64" t="s">
         <v>517</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
@@ -9700,12 +9706,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B1:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E23" r:id="rId1" display="https://creativecommons.org/licenses/by-nc-sa/3.0/igo" xr:uid="{3F70E5F0-79E0-4591-82A3-7482398AC806}"/>
@@ -9721,21 +9721,21 @@
   <dimension ref="A1:Z172"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="44" style="5" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="81.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="59.85546875" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="3" max="3" width="42.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="74.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="81.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="59.83203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="18" customFormat="1">
+    <row r="2" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>336</v>
       </c>
@@ -9765,7 +9765,7 @@
       <c r="E2" s="28"/>
       <c r="F2" s="29"/>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1">
+    <row r="3" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>4</v>
       </c>
@@ -9795,7 +9795,7 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="9"/>
     </row>
-    <row r="4" spans="1:26" s="4" customFormat="1">
+    <row r="4" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>5</v>
       </c>
@@ -9833,7 +9833,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" s="4" customFormat="1">
+    <row r="5" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>8</v>
       </c>
@@ -9871,7 +9871,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
         <v>9</v>
       </c>
@@ -9889,7 +9889,7 @@
       </c>
       <c r="F6" s="35"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
         <v>10</v>
       </c>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="F7" s="35"/>
     </row>
-    <row r="8" spans="1:26" ht="26.25">
+    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
         <v>12</v>
       </c>
@@ -9925,7 +9925,7 @@
       </c>
       <c r="F8" s="35"/>
     </row>
-    <row r="9" spans="1:26" ht="25.5">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
         <v>13</v>
       </c>
@@ -9943,7 +9943,7 @@
       </c>
       <c r="F9" s="35"/>
     </row>
-    <row r="10" spans="1:26" ht="26.25">
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
         <v>15</v>
       </c>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="F10" s="35"/>
     </row>
-    <row r="11" spans="1:26" ht="26.25">
+    <row r="11" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>17</v>
       </c>
@@ -9979,7 +9979,7 @@
       </c>
       <c r="F11" s="35"/>
     </row>
-    <row r="12" spans="1:26" ht="26.25">
+    <row r="12" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
         <v>18</v>
       </c>
@@ -9997,7 +9997,7 @@
       </c>
       <c r="F12" s="35"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
         <v>20</v>
       </c>
@@ -10015,7 +10015,7 @@
       </c>
       <c r="F13" s="35"/>
     </row>
-    <row r="14" spans="1:26" ht="26.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
         <v>23</v>
       </c>
@@ -10033,7 +10033,7 @@
       </c>
       <c r="F14" s="35"/>
     </row>
-    <row r="15" spans="1:26" ht="26.25">
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
         <v>25</v>
       </c>
@@ -10051,7 +10051,7 @@
       </c>
       <c r="F15" s="35"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
         <v>26</v>
       </c>
@@ -10069,7 +10069,7 @@
       </c>
       <c r="F16" s="35"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="36"/>
       <c r="B17" s="37" t="s">
         <v>358</v>
@@ -10085,7 +10085,7 @@
       </c>
       <c r="F17" s="35"/>
     </row>
-    <row r="18" spans="1:6" ht="26.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
         <v>28</v>
       </c>
@@ -10103,7 +10103,7 @@
       </c>
       <c r="F18" s="35"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
         <v>31</v>
       </c>
@@ -10121,7 +10121,7 @@
       </c>
       <c r="F19" s="35"/>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
         <v>34</v>
       </c>
@@ -10139,7 +10139,7 @@
       </c>
       <c r="F20" s="35"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
         <v>36</v>
       </c>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="F21" s="35"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
         <v>39</v>
       </c>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="F22" s="35"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
         <v>42</v>
       </c>
@@ -10193,7 +10193,7 @@
       </c>
       <c r="F23" s="35"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="33"/>
       <c r="B24" s="37" t="s">
         <v>45</v>
@@ -10209,7 +10209,7 @@
       </c>
       <c r="F24" s="35"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
         <v>46</v>
       </c>
@@ -10227,7 +10227,7 @@
       </c>
       <c r="F25" s="35"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
         <v>49</v>
       </c>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="F26" s="35"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
         <v>50</v>
       </c>
@@ -10263,7 +10263,7 @@
       </c>
       <c r="F27" s="35"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
         <v>51</v>
       </c>
@@ -10281,7 +10281,7 @@
       </c>
       <c r="F28" s="35"/>
     </row>
-    <row r="29" spans="1:6" s="10" customFormat="1" ht="26.25">
+    <row r="29" spans="1:6" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
         <v>52</v>
       </c>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="F29" s="35"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
         <v>54</v>
       </c>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="F30" s="35"/>
     </row>
-    <row r="31" spans="1:6" ht="26.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
         <v>58</v>
       </c>
@@ -10335,7 +10335,7 @@
       </c>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
         <v>59</v>
       </c>
@@ -10353,7 +10353,7 @@
       </c>
       <c r="F32" s="35"/>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
         <v>62</v>
       </c>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="F33" s="35"/>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
         <v>64</v>
       </c>
@@ -10389,7 +10389,7 @@
       </c>
       <c r="F34" s="35"/>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
         <v>66</v>
       </c>
@@ -10407,7 +10407,7 @@
       </c>
       <c r="F35" s="35"/>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
         <v>69</v>
       </c>
@@ -10425,7 +10425,7 @@
       </c>
       <c r="F36" s="35"/>
     </row>
-    <row r="37" spans="1:26" s="18" customFormat="1">
+    <row r="37" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="s">
         <v>371</v>
       </c>
@@ -10435,7 +10435,7 @@
       <c r="E37" s="28"/>
       <c r="F37" s="29"/>
     </row>
-    <row r="38" spans="1:26" s="2" customFormat="1">
+    <row r="38" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>72</v>
       </c>
@@ -10465,7 +10465,7 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="9"/>
     </row>
-    <row r="39" spans="1:26" s="14" customFormat="1">
+    <row r="39" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
         <v>5</v>
       </c>
@@ -10503,7 +10503,7 @@
       <c r="Y39" s="13"/>
       <c r="Z39" s="13"/>
     </row>
-    <row r="40" spans="1:26" s="14" customFormat="1">
+    <row r="40" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
         <v>8</v>
       </c>
@@ -10541,7 +10541,7 @@
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
         <v>9</v>
       </c>
@@ -10559,7 +10559,7 @@
       </c>
       <c r="F41" s="35"/>
     </row>
-    <row r="42" spans="1:26" ht="26.25">
+    <row r="42" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
         <v>10</v>
       </c>
@@ -10577,7 +10577,7 @@
       </c>
       <c r="F42" s="35"/>
     </row>
-    <row r="43" spans="1:26" ht="26.25">
+    <row r="43" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
         <v>12</v>
       </c>
@@ -10595,7 +10595,7 @@
       </c>
       <c r="F43" s="35"/>
     </row>
-    <row r="44" spans="1:26" ht="51.75">
+    <row r="44" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
         <v>13</v>
       </c>
@@ -10613,7 +10613,7 @@
       </c>
       <c r="F44" s="35"/>
     </row>
-    <row r="45" spans="1:26" ht="26.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
         <v>15</v>
       </c>
@@ -10631,7 +10631,7 @@
       </c>
       <c r="F45" s="35"/>
     </row>
-    <row r="46" spans="1:26" ht="26.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="33" t="s">
         <v>17</v>
       </c>
@@ -10649,7 +10649,7 @@
       </c>
       <c r="F46" s="35"/>
     </row>
-    <row r="47" spans="1:26" ht="26.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="33" t="s">
         <v>18</v>
       </c>
@@ -10667,7 +10667,7 @@
       </c>
       <c r="F47" s="35"/>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="33" t="s">
         <v>20</v>
       </c>
@@ -10685,7 +10685,7 @@
       </c>
       <c r="F48" s="35"/>
     </row>
-    <row r="49" spans="1:6" ht="26.25">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="33" t="s">
         <v>23</v>
       </c>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="F49" s="35"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="33"/>
       <c r="B50" s="37" t="s">
         <v>384</v>
@@ -10719,7 +10719,7 @@
       </c>
       <c r="F50" s="35"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="33"/>
       <c r="B51" s="37" t="s">
         <v>386</v>
@@ -10735,7 +10735,7 @@
       </c>
       <c r="F51" s="35"/>
     </row>
-    <row r="52" spans="1:6" ht="26.25">
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="33" t="s">
         <v>25</v>
       </c>
@@ -10753,7 +10753,7 @@
       </c>
       <c r="F52" s="35"/>
     </row>
-    <row r="53" spans="1:6" ht="26.25">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="33" t="s">
         <v>26</v>
       </c>
@@ -10771,7 +10771,7 @@
       </c>
       <c r="F53" s="35"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
       <c r="B54" s="37" t="s">
         <v>88</v>
@@ -10787,7 +10787,7 @@
       </c>
       <c r="F54" s="35"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="33" t="s">
         <v>28</v>
       </c>
@@ -10805,7 +10805,7 @@
       </c>
       <c r="F55" s="35"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="33" t="s">
         <v>31</v>
       </c>
@@ -10823,7 +10823,7 @@
       </c>
       <c r="F56" s="35"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
         <v>34</v>
       </c>
@@ -10841,7 +10841,7 @@
       </c>
       <c r="F57" s="35"/>
     </row>
-    <row r="58" spans="1:6" ht="26.25">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A58" s="33" t="s">
         <v>36</v>
       </c>
@@ -10859,7 +10859,7 @@
       </c>
       <c r="F58" s="35"/>
     </row>
-    <row r="59" spans="1:6" ht="51.75">
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="33" t="s">
         <v>39</v>
       </c>
@@ -10877,7 +10877,7 @@
       </c>
       <c r="F59" s="35"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="33" t="s">
         <v>42</v>
       </c>
@@ -10895,7 +10895,7 @@
       </c>
       <c r="F60" s="35"/>
     </row>
-    <row r="61" spans="1:6" ht="26.25">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="33" t="s">
         <v>46</v>
       </c>
@@ -10913,7 +10913,7 @@
       </c>
       <c r="F61" s="35"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="33" t="s">
         <v>49</v>
       </c>
@@ -10931,7 +10931,7 @@
       </c>
       <c r="F62" s="35"/>
     </row>
-    <row r="63" spans="1:6" ht="26.25">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="33" t="s">
         <v>50</v>
       </c>
@@ -10949,7 +10949,7 @@
       </c>
       <c r="F63" s="35"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="33"/>
       <c r="B64" s="37" t="s">
         <v>102</v>
@@ -10965,7 +10965,7 @@
       </c>
       <c r="F64" s="35"/>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="33" t="s">
         <v>51</v>
       </c>
@@ -10983,7 +10983,7 @@
       </c>
       <c r="F65" s="35"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="33" t="s">
         <v>52</v>
       </c>
@@ -11001,7 +11001,7 @@
       </c>
       <c r="F66" s="35"/>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="33" t="s">
         <v>54</v>
       </c>
@@ -11019,7 +11019,7 @@
       </c>
       <c r="F67" s="35"/>
     </row>
-    <row r="68" spans="1:26" ht="26.25">
+    <row r="68" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="33" t="s">
         <v>58</v>
       </c>
@@ -11037,7 +11037,7 @@
       </c>
       <c r="F68" s="35"/>
     </row>
-    <row r="69" spans="1:26">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="33" t="s">
         <v>59</v>
       </c>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="F69" s="35"/>
     </row>
-    <row r="70" spans="1:26">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="33" t="s">
         <v>62</v>
       </c>
@@ -11073,7 +11073,7 @@
       </c>
       <c r="F70" s="35"/>
     </row>
-    <row r="71" spans="1:26">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="33" t="s">
         <v>64</v>
       </c>
@@ -11091,7 +11091,7 @@
       </c>
       <c r="F71" s="35"/>
     </row>
-    <row r="72" spans="1:26" ht="26.25">
+    <row r="72" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" s="33" t="s">
         <v>66</v>
       </c>
@@ -11109,7 +11109,7 @@
       </c>
       <c r="F72" s="35"/>
     </row>
-    <row r="73" spans="1:26" s="18" customFormat="1">
+    <row r="73" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
         <v>398</v>
       </c>
@@ -11119,7 +11119,7 @@
       <c r="E73" s="28"/>
       <c r="F73" s="29"/>
     </row>
-    <row r="74" spans="1:26" s="24" customFormat="1">
+    <row r="74" spans="1:26" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="40" t="s">
         <v>399</v>
       </c>
@@ -11149,7 +11149,7 @@
       <c r="Y74" s="22"/>
       <c r="Z74" s="23"/>
     </row>
-    <row r="75" spans="1:26">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="33" t="s">
         <v>5</v>
       </c>
@@ -11167,7 +11167,7 @@
       </c>
       <c r="F75" s="35"/>
     </row>
-    <row r="76" spans="1:26">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="35"/>
       <c r="B76" s="37" t="s">
         <v>105</v>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="F76" s="35"/>
     </row>
-    <row r="77" spans="1:26" ht="25.5">
+    <row r="77" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="33" t="s">
         <v>8</v>
       </c>
@@ -11201,7 +11201,7 @@
       </c>
       <c r="F77" s="35"/>
     </row>
-    <row r="78" spans="1:26">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="33" t="s">
         <v>9</v>
       </c>
@@ -11219,7 +11219,7 @@
       </c>
       <c r="F78" s="35"/>
     </row>
-    <row r="79" spans="1:26" ht="26.25">
+    <row r="79" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="33" t="s">
         <v>10</v>
       </c>
@@ -11237,7 +11237,7 @@
       </c>
       <c r="F79" s="35"/>
     </row>
-    <row r="80" spans="1:26" ht="26.25">
+    <row r="80" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="33" t="s">
         <v>12</v>
       </c>
@@ -11255,7 +11255,7 @@
       </c>
       <c r="F80" s="35"/>
     </row>
-    <row r="81" spans="1:6" ht="26.25">
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="33" t="s">
         <v>13</v>
       </c>
@@ -11273,7 +11273,7 @@
       </c>
       <c r="F81" s="35"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="33" t="s">
         <v>15</v>
       </c>
@@ -11291,7 +11291,7 @@
       </c>
       <c r="F82" s="35"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="33" t="s">
         <v>17</v>
       </c>
@@ -11309,7 +11309,7 @@
       </c>
       <c r="F83" s="35"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="33" t="s">
         <v>18</v>
       </c>
@@ -11327,7 +11327,7 @@
       </c>
       <c r="F84" s="35"/>
     </row>
-    <row r="85" spans="1:6" ht="26.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A85" s="33" t="s">
         <v>20</v>
       </c>
@@ -11345,7 +11345,7 @@
       </c>
       <c r="F85" s="35"/>
     </row>
-    <row r="86" spans="1:6" ht="26.25">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="33" t="s">
         <v>23</v>
       </c>
@@ -11363,7 +11363,7 @@
       </c>
       <c r="F86" s="35"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="33"/>
       <c r="B87" s="37" t="s">
         <v>411</v>
@@ -11379,7 +11379,7 @@
       </c>
       <c r="F87" s="35"/>
     </row>
-    <row r="88" spans="1:6" ht="26.25">
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A88" s="33" t="s">
         <v>25</v>
       </c>
@@ -11397,7 +11397,7 @@
       </c>
       <c r="F88" s="35"/>
     </row>
-    <row r="89" spans="1:6" ht="26.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="33" t="s">
         <v>26</v>
       </c>
@@ -11415,7 +11415,7 @@
       </c>
       <c r="F89" s="35"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="33" t="s">
         <v>28</v>
       </c>
@@ -11433,7 +11433,7 @@
       </c>
       <c r="F90" s="35"/>
     </row>
-    <row r="91" spans="1:6" ht="26.25">
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="33" t="s">
         <v>31</v>
       </c>
@@ -11451,7 +11451,7 @@
       </c>
       <c r="F91" s="35"/>
     </row>
-    <row r="92" spans="1:6" ht="26.25">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="33" t="s">
         <v>34</v>
       </c>
@@ -11469,7 +11469,7 @@
       </c>
       <c r="F92" s="35"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="33" t="s">
         <v>36</v>
       </c>
@@ -11487,7 +11487,7 @@
       </c>
       <c r="F93" s="35"/>
     </row>
-    <row r="94" spans="1:6" ht="26.25">
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="33" t="s">
         <v>39</v>
       </c>
@@ -11505,7 +11505,7 @@
       </c>
       <c r="F94" s="35"/>
     </row>
-    <row r="95" spans="1:6" ht="26.25">
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="33" t="s">
         <v>42</v>
       </c>
@@ -11523,7 +11523,7 @@
       </c>
       <c r="F95" s="35"/>
     </row>
-    <row r="96" spans="1:6" ht="26.25">
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="33" t="s">
         <v>46</v>
       </c>
@@ -11541,7 +11541,7 @@
       </c>
       <c r="F96" s="35"/>
     </row>
-    <row r="97" spans="1:26" ht="26.25">
+    <row r="97" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A97" s="33" t="s">
         <v>49</v>
       </c>
@@ -11559,7 +11559,7 @@
       </c>
       <c r="F97" s="35"/>
     </row>
-    <row r="98" spans="1:26" s="18" customFormat="1">
+    <row r="98" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="44" t="s">
         <v>416</v>
       </c>
@@ -11569,7 +11569,7 @@
       <c r="E98" s="28"/>
       <c r="F98" s="29"/>
     </row>
-    <row r="99" spans="1:26" s="2" customFormat="1">
+    <row r="99" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="30" t="s">
         <v>118</v>
       </c>
@@ -11599,7 +11599,7 @@
       <c r="Y99" s="8"/>
       <c r="Z99" s="9"/>
     </row>
-    <row r="100" spans="1:26">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="33" t="s">
         <v>5</v>
       </c>
@@ -11617,7 +11617,7 @@
       </c>
       <c r="F100" s="35"/>
     </row>
-    <row r="101" spans="1:26">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="33"/>
       <c r="B101" s="37" t="s">
         <v>418</v>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="F101" s="35"/>
     </row>
-    <row r="102" spans="1:26" ht="26.25">
+    <row r="102" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A102" s="33" t="s">
         <v>8</v>
       </c>
@@ -11651,7 +11651,7 @@
       </c>
       <c r="F102" s="35"/>
     </row>
-    <row r="103" spans="1:26">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="33"/>
       <c r="B103" s="37" t="s">
         <v>421</v>
@@ -11667,7 +11667,7 @@
       </c>
       <c r="F103" s="35"/>
     </row>
-    <row r="104" spans="1:26">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="33" t="s">
         <v>9</v>
       </c>
@@ -11685,7 +11685,7 @@
       </c>
       <c r="F104" s="35"/>
     </row>
-    <row r="105" spans="1:26">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="33" t="s">
         <v>10</v>
       </c>
@@ -11703,7 +11703,7 @@
       </c>
       <c r="F105" s="35"/>
     </row>
-    <row r="106" spans="1:26">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="33" t="s">
         <v>12</v>
       </c>
@@ -11721,7 +11721,7 @@
       </c>
       <c r="F106" s="35"/>
     </row>
-    <row r="107" spans="1:26">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="33" t="s">
         <v>13</v>
       </c>
@@ -11739,7 +11739,7 @@
       </c>
       <c r="F107" s="35"/>
     </row>
-    <row r="108" spans="1:26">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="33" t="s">
         <v>15</v>
       </c>
@@ -11757,7 +11757,7 @@
       </c>
       <c r="F108" s="35"/>
     </row>
-    <row r="109" spans="1:26">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="33" t="s">
         <v>17</v>
       </c>
@@ -11775,7 +11775,7 @@
       </c>
       <c r="F109" s="35"/>
     </row>
-    <row r="110" spans="1:26">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="33" t="s">
         <v>18</v>
       </c>
@@ -11793,7 +11793,7 @@
       </c>
       <c r="F110" s="35"/>
     </row>
-    <row r="111" spans="1:26">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="33" t="s">
         <v>20</v>
       </c>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="F111" s="35"/>
     </row>
-    <row r="112" spans="1:26">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="33" t="s">
         <v>23</v>
       </c>
@@ -11829,7 +11829,7 @@
       </c>
       <c r="F112" s="35"/>
     </row>
-    <row r="113" spans="1:26">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="33" t="s">
         <v>25</v>
       </c>
@@ -11847,7 +11847,7 @@
       </c>
       <c r="F113" s="35"/>
     </row>
-    <row r="114" spans="1:26" ht="26.25">
+    <row r="114" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A114" s="33" t="s">
         <v>26</v>
       </c>
@@ -11865,7 +11865,7 @@
       </c>
       <c r="F114" s="35"/>
     </row>
-    <row r="115" spans="1:26">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="33" t="s">
         <v>28</v>
       </c>
@@ -11883,7 +11883,7 @@
       </c>
       <c r="F115" s="35"/>
     </row>
-    <row r="116" spans="1:26">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="33" t="s">
         <v>31</v>
       </c>
@@ -11901,7 +11901,7 @@
       </c>
       <c r="F116" s="35"/>
     </row>
-    <row r="117" spans="1:26">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="33" t="s">
         <v>34</v>
       </c>
@@ -11919,7 +11919,7 @@
       </c>
       <c r="F117" s="35"/>
     </row>
-    <row r="118" spans="1:26">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="33" t="s">
         <v>36</v>
       </c>
@@ -11937,7 +11937,7 @@
       </c>
       <c r="F118" s="35"/>
     </row>
-    <row r="119" spans="1:26" s="18" customFormat="1">
+    <row r="119" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="27" t="s">
         <v>440</v>
       </c>
@@ -11947,7 +11947,7 @@
       <c r="E119" s="28"/>
       <c r="F119" s="29"/>
     </row>
-    <row r="120" spans="1:26" s="2" customFormat="1">
+    <row r="120" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="45" t="s">
         <v>441</v>
       </c>
@@ -11977,7 +11977,7 @@
       <c r="Y120" s="8"/>
       <c r="Z120" s="9"/>
     </row>
-    <row r="121" spans="1:26" s="4" customFormat="1">
+    <row r="121" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="33" t="s">
         <v>5</v>
       </c>
@@ -12015,7 +12015,7 @@
       <c r="Y121" s="6"/>
       <c r="Z121" s="6"/>
     </row>
-    <row r="122" spans="1:26">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122" s="33"/>
       <c r="B122" s="37" t="s">
         <v>445</v>
@@ -12029,7 +12029,7 @@
       <c r="E122" s="35"/>
       <c r="F122" s="35"/>
     </row>
-    <row r="123" spans="1:26">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123" s="33" t="s">
         <v>8</v>
       </c>
@@ -12047,7 +12047,7 @@
       </c>
       <c r="F123" s="35"/>
     </row>
-    <row r="124" spans="1:26">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="33" t="s">
         <v>9</v>
       </c>
@@ -12065,7 +12065,7 @@
       </c>
       <c r="F124" s="35"/>
     </row>
-    <row r="125" spans="1:26">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="33" t="s">
         <v>10</v>
       </c>
@@ -12083,7 +12083,7 @@
       </c>
       <c r="F125" s="35"/>
     </row>
-    <row r="126" spans="1:26">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="33" t="s">
         <v>12</v>
       </c>
@@ -12101,7 +12101,7 @@
       </c>
       <c r="F126" s="35"/>
     </row>
-    <row r="127" spans="1:26">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127" s="33" t="s">
         <v>13</v>
       </c>
@@ -12119,7 +12119,7 @@
       </c>
       <c r="F127" s="35"/>
     </row>
-    <row r="128" spans="1:26" ht="26.25">
+    <row r="128" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A128" s="33" t="s">
         <v>15</v>
       </c>
@@ -12137,7 +12137,7 @@
       </c>
       <c r="F128" s="35"/>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="33" t="s">
         <v>17</v>
       </c>
@@ -12155,7 +12155,7 @@
       </c>
       <c r="F129" s="35"/>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="33" t="s">
         <v>18</v>
       </c>
@@ -12173,7 +12173,7 @@
       </c>
       <c r="F130" s="35"/>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="33"/>
       <c r="B131" s="37" t="s">
         <v>454</v>
@@ -12189,7 +12189,7 @@
       </c>
       <c r="F131" s="35"/>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="33" t="s">
         <v>20</v>
       </c>
@@ -12207,7 +12207,7 @@
       </c>
       <c r="F132" s="35"/>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="33" t="s">
         <v>23</v>
       </c>
@@ -12225,7 +12225,7 @@
       </c>
       <c r="F133" s="35"/>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="33" t="s">
         <v>25</v>
       </c>
@@ -12243,7 +12243,7 @@
       </c>
       <c r="F134" s="35"/>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="33" t="s">
         <v>26</v>
       </c>
@@ -12261,7 +12261,7 @@
       </c>
       <c r="F135" s="35"/>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="33" t="s">
         <v>28</v>
       </c>
@@ -12279,7 +12279,7 @@
       </c>
       <c r="F136" s="35"/>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="33" t="s">
         <v>31</v>
       </c>
@@ -12297,7 +12297,7 @@
       </c>
       <c r="F137" s="35"/>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="33" t="s">
         <v>34</v>
       </c>
@@ -12315,7 +12315,7 @@
       </c>
       <c r="F138" s="35"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A139" s="33" t="s">
         <v>36</v>
       </c>
@@ -12333,7 +12333,7 @@
       </c>
       <c r="F139" s="35"/>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="33" t="s">
         <v>39</v>
       </c>
@@ -12351,7 +12351,7 @@
       </c>
       <c r="F140" s="35"/>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="33" t="s">
         <v>42</v>
       </c>
@@ -12369,7 +12369,7 @@
       </c>
       <c r="F141" s="35"/>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="33" t="s">
         <v>46</v>
       </c>
@@ -12387,7 +12387,7 @@
       </c>
       <c r="F142" s="35"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="33" t="s">
         <v>49</v>
       </c>
@@ -12405,7 +12405,7 @@
       </c>
       <c r="F143" s="35"/>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="33" t="s">
         <v>50</v>
       </c>
@@ -12423,7 +12423,7 @@
       </c>
       <c r="F144" s="35"/>
     </row>
-    <row r="145" spans="1:26" ht="26.25">
+    <row r="145" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A145" s="33" t="s">
         <v>51</v>
       </c>
@@ -12441,7 +12441,7 @@
       </c>
       <c r="F145" s="35"/>
     </row>
-    <row r="146" spans="1:26" s="18" customFormat="1">
+    <row r="146" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="44" t="s">
         <v>148</v>
       </c>
@@ -12451,7 +12451,7 @@
       <c r="E146" s="28"/>
       <c r="F146" s="29"/>
     </row>
-    <row r="147" spans="1:26" s="2" customFormat="1">
+    <row r="147" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="30" t="s">
         <v>149</v>
       </c>
@@ -12481,7 +12481,7 @@
       <c r="Y147" s="8"/>
       <c r="Z147" s="9"/>
     </row>
-    <row r="148" spans="1:26" ht="26.25">
+    <row r="148" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A148" s="33" t="s">
         <v>5</v>
       </c>
@@ -12499,7 +12499,7 @@
       </c>
       <c r="F148" s="35"/>
     </row>
-    <row r="149" spans="1:26" ht="26.25">
+    <row r="149" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A149" s="33" t="s">
         <v>8</v>
       </c>
@@ -12517,7 +12517,7 @@
       </c>
       <c r="F149" s="35"/>
     </row>
-    <row r="150" spans="1:26" ht="39">
+    <row r="150" spans="1:26" ht="45" x14ac:dyDescent="0.2">
       <c r="A150" s="33" t="s">
         <v>9</v>
       </c>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="F150" s="35"/>
     </row>
-    <row r="151" spans="1:26" s="18" customFormat="1">
+    <row r="151" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="27" t="s">
         <v>473</v>
       </c>
@@ -12545,7 +12545,7 @@
       <c r="E151" s="28"/>
       <c r="F151" s="29"/>
     </row>
-    <row r="152" spans="1:26" s="2" customFormat="1">
+    <row r="152" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="30" t="s">
         <v>155</v>
       </c>
@@ -12575,7 +12575,7 @@
       <c r="Y152" s="8"/>
       <c r="Z152" s="9"/>
     </row>
-    <row r="153" spans="1:26">
+    <row r="153" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A153" s="33" t="s">
         <v>5</v>
       </c>
@@ -12591,7 +12591,7 @@
       <c r="E153" s="35"/>
       <c r="F153" s="35"/>
     </row>
-    <row r="154" spans="1:26">
+    <row r="154" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A154" s="33" t="s">
         <v>8</v>
       </c>
@@ -12609,7 +12609,7 @@
       </c>
       <c r="F154" s="35"/>
     </row>
-    <row r="155" spans="1:26">
+    <row r="155" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A155" s="33" t="s">
         <v>9</v>
       </c>
@@ -12627,7 +12627,7 @@
       </c>
       <c r="F155" s="35"/>
     </row>
-    <row r="156" spans="1:26" ht="26.25">
+    <row r="156" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A156" s="33" t="s">
         <v>10</v>
       </c>
@@ -12645,7 +12645,7 @@
       </c>
       <c r="F156" s="35"/>
     </row>
-    <row r="157" spans="1:26" s="12" customFormat="1">
+    <row r="157" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="47" t="s">
         <v>478</v>
       </c>
@@ -12655,7 +12655,7 @@
       <c r="E157" s="47"/>
       <c r="F157" s="47"/>
     </row>
-    <row r="158" spans="1:26" ht="26.25">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158" s="33" t="s">
         <v>5</v>
       </c>
@@ -12673,7 +12673,7 @@
       </c>
       <c r="F158" s="35"/>
     </row>
-    <row r="159" spans="1:26" ht="90">
+    <row r="159" spans="1:26" ht="75" x14ac:dyDescent="0.2">
       <c r="A159" s="33" t="s">
         <v>8</v>
       </c>
@@ -12691,7 +12691,7 @@
       </c>
       <c r="F159" s="35"/>
     </row>
-    <row r="160" spans="1:26" ht="39">
+    <row r="160" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A160" s="33" t="s">
         <v>9</v>
       </c>
@@ -12709,7 +12709,7 @@
       </c>
       <c r="F160" s="35"/>
     </row>
-    <row r="161" spans="1:6" ht="39">
+    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A161" s="33" t="s">
         <v>10</v>
       </c>
@@ -12727,7 +12727,7 @@
       </c>
       <c r="F161" s="35"/>
     </row>
-    <row r="162" spans="1:6" ht="26.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="33" t="s">
         <v>12</v>
       </c>
@@ -12745,7 +12745,7 @@
       </c>
       <c r="F162" s="35"/>
     </row>
-    <row r="163" spans="1:6" ht="26.25">
+    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A163" s="33" t="s">
         <v>13</v>
       </c>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="F163" s="35"/>
     </row>
-    <row r="164" spans="1:6" ht="26.25">
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A164" s="33" t="s">
         <v>15</v>
       </c>
@@ -12781,7 +12781,7 @@
       </c>
       <c r="F164" s="35"/>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="33" t="s">
         <v>17</v>
       </c>
@@ -12799,7 +12799,7 @@
       </c>
       <c r="F165" s="35"/>
     </row>
-    <row r="166" spans="1:6" ht="39">
+    <row r="166" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A166" s="33" t="s">
         <v>18</v>
       </c>
@@ -12817,7 +12817,7 @@
       </c>
       <c r="F166" s="35"/>
     </row>
-    <row r="167" spans="1:6" ht="39">
+    <row r="167" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A167" s="33" t="s">
         <v>20</v>
       </c>
@@ -12835,7 +12835,7 @@
       </c>
       <c r="F167" s="35"/>
     </row>
-    <row r="168" spans="1:6" ht="39">
+    <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A168" s="33" t="s">
         <v>23</v>
       </c>
@@ -12853,7 +12853,7 @@
       </c>
       <c r="F168" s="35"/>
     </row>
-    <row r="169" spans="1:6" ht="39">
+    <row r="169" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A169" s="33" t="s">
         <v>25</v>
       </c>
@@ -12871,7 +12871,7 @@
       </c>
       <c r="F169" s="35"/>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -12879,7 +12879,7 @@
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -12887,7 +12887,7 @@
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
     </row>
-    <row r="172" spans="1:6" s="15" customFormat="1">
+    <row r="172" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="11"/>
       <c r="C172" s="11"/>
@@ -12905,41 +12905,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE5B051-F32D-41A1-B37F-742ED587C451}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="244" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B12" sqref="B12"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="131.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="131.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="18" customFormat="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>497</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
         <v>175</v>
       </c>
@@ -12950,7 +12950,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>178</v>
       </c>
@@ -12961,7 +12961,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>180</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="51" t="s">
         <v>182</v>
       </c>
@@ -12983,7 +12983,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="51" t="s">
         <v>184</v>
       </c>
@@ -12994,7 +12994,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
         <v>186</v>
       </c>
@@ -13005,7 +13005,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
         <v>188</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>190</v>
       </c>
@@ -13027,7 +13027,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>193</v>
       </c>
@@ -13038,7 +13038,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
         <v>195</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="51" t="s">
         <v>197</v>
       </c>
@@ -13060,7 +13060,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>199</v>
       </c>
@@ -13071,7 +13071,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>201</v>
       </c>
@@ -13082,7 +13082,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>203</v>
       </c>
@@ -13093,7 +13093,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
         <v>205</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
         <v>207</v>
       </c>
@@ -13115,7 +13115,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="51" t="s">
         <v>210</v>
       </c>
@@ -13126,7 +13126,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="51" t="s">
         <v>212</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="51" t="s">
         <v>214</v>
       </c>
@@ -13148,7 +13148,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>216</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="51" t="s">
         <v>218</v>
       </c>
@@ -13170,7 +13170,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
         <v>220</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="51" t="s">
         <v>221</v>
       </c>
@@ -13192,7 +13192,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="51" t="s">
         <v>223</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="51" t="s">
         <v>226</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" customHeight="1">
+    <row r="28" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="51" t="s">
         <v>228</v>
       </c>
@@ -13225,7 +13225,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="51" t="s">
         <v>229</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="51" t="s">
         <v>231</v>
       </c>
@@ -13247,7 +13247,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="51" t="s">
         <v>233</v>
       </c>
@@ -13258,7 +13258,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="51" t="s">
         <v>235</v>
       </c>
@@ -13269,7 +13269,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="51" t="s">
         <v>237</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="51" t="s">
         <v>239</v>
       </c>
@@ -13291,7 +13291,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="51" t="s">
         <v>241</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="51" t="s">
         <v>243</v>
       </c>
@@ -13313,7 +13313,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="51" t="s">
         <v>246</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="51" t="s">
         <v>248</v>
       </c>
@@ -13335,7 +13335,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="51" t="s">
         <v>250</v>
       </c>
@@ -13346,7 +13346,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="51" t="s">
         <v>252</v>
       </c>
@@ -13357,7 +13357,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="51" t="s">
         <v>254</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="51" t="s">
         <v>256</v>
       </c>
@@ -13379,7 +13379,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="51" t="s">
         <v>258</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
         <v>260</v>
       </c>
@@ -13401,7 +13401,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
         <v>262</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="51" t="s">
         <v>264</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
         <v>266</v>
       </c>
@@ -13434,7 +13434,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
         <v>268</v>
       </c>
@@ -13445,7 +13445,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="51" t="s">
         <v>271</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="51" t="s">
         <v>273</v>
       </c>
@@ -13467,7 +13467,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="51" t="s">
         <v>275</v>
       </c>
@@ -13478,7 +13478,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="51" t="s">
         <v>277</v>
       </c>
@@ -13489,7 +13489,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="51" t="s">
         <v>280</v>
       </c>
@@ -13500,7 +13500,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="51" t="s">
         <v>282</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
         <v>284</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="51" t="s">
         <v>286</v>
       </c>
@@ -13533,7 +13533,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="51" t="s">
         <v>288</v>
       </c>
@@ -13544,7 +13544,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="51" t="s">
         <v>290</v>
       </c>
@@ -13555,7 +13555,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="51" t="s">
         <v>292</v>
       </c>
@@ -13566,7 +13566,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="51" t="s">
         <v>294</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="51" t="s">
         <v>296</v>
       </c>
@@ -13588,7 +13588,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="51" t="s">
         <v>298</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="51" t="s">
         <v>300</v>
       </c>
@@ -13610,7 +13610,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="25.5">
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="51" t="s">
         <v>303</v>
       </c>
@@ -13621,7 +13621,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="51" t="s">
         <v>305</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="51" t="s">
         <v>307</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="51" t="s">
         <v>309</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="25.5">
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="51" t="s">
         <v>312</v>
       </c>
@@ -13665,7 +13665,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="51" t="s">
         <v>314</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="51" t="s">
         <v>316</v>
       </c>
@@ -13687,7 +13687,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="51" t="s">
         <v>318</v>
       </c>
@@ -13698,7 +13698,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="51" t="s">
         <v>320</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
         <v>322</v>
       </c>
@@ -13720,7 +13720,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25.5">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="51" t="s">
         <v>324</v>
       </c>
@@ -13731,7 +13731,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="51" t="s">
         <v>327</v>
       </c>
@@ -13742,7 +13742,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="51" t="s">
         <v>329</v>
       </c>
@@ -13753,7 +13753,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="25.5">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="51" t="s">
         <v>331</v>
       </c>
@@ -13771,26 +13771,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="416825ba-b8fd-4a6e-a018-bb0771c19d68" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d65e7f8b-cc59-4424-bfae-3a1bbee13083">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010041B804C18649484BAB55685C5273DA06" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61894d8f9c4b190eee51c0cf06c995e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d65e7f8b-cc59-4424-bfae-3a1bbee13083" xmlns:ns3="416825ba-b8fd-4a6e-a018-bb0771c19d68" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="096c4ea54889fea4cccfa426c4799a2c" ns2:_="" ns3:_="">
     <xsd:import namespace="d65e7f8b-cc59-4424-bfae-3a1bbee13083"/>
@@ -14039,10 +14019,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="416825ba-b8fd-4a6e-a018-bb0771c19d68" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d65e7f8b-cc59-4424-bfae-3a1bbee13083">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99DD44E-BE83-4250-829F-7CDFCD4908BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8647B294-18FF-411B-88D9-47EBEA5E471D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d65e7f8b-cc59-4424-bfae-3a1bbee13083"/>
+    <ds:schemaRef ds:uri="416825ba-b8fd-4a6e-a018-bb0771c19d68"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14065,20 +14076,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8647B294-18FF-411B-88D9-47EBEA5E471D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99DD44E-BE83-4250-829F-7CDFCD4908BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d65e7f8b-cc59-4424-bfae-3a1bbee13083"/>
-    <ds:schemaRef ds:uri="416825ba-b8fd-4a6e-a018-bb0771c19d68"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>